<commit_message>
feat(jeu des jetons): Ajuster l'énoncé
</commit_message>
<xml_diff>
--- a/Matériel/Jeu des pièces.xlsx
+++ b/Matériel/Jeu des pièces.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Xavier/Github/ICT-306/Matériel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Xavier/Github/ICT-306/Matériel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58AFBBAC-00D4-BF4A-A547-BBBF2FAEF47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC653D97-F80D-294E-89FD-8347E6F23F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{EE96F8C1-1BF4-964D-BC6C-8FC8595EF899}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Temps</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>bleus de valeur</t>
+  </si>
+  <si>
+    <t>verts de valeur</t>
+  </si>
+  <si>
+    <t>rouges de valeur</t>
   </si>
 </sst>
 </file>
@@ -129,13 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -146,7 +152,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5163,9 +5171,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5203,7 +5211,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5309,7 +5317,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5451,7 +5459,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5462,7 +5470,7 @@
   <dimension ref="A1:P93"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5474,30 +5482,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="A3" s="5"/>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
         <v>0</v>
       </c>
       <c r="N3" t="s">
@@ -5505,33 +5513,33 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="A4" s="5"/>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="P4">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="A5" s="5"/>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O5" t="s">
         <v>8</v>
@@ -5541,57 +5549,56 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="L6" s="6"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
       <c r="N6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="P6">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="4">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="P7">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="4">
-        <v>0</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="A8" s="5"/>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4">
-        <v>0</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="A9" s="5"/>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
         <v>0</v>
       </c>
       <c r="O9" t="s">
@@ -5599,698 +5606,694 @@
       </c>
       <c r="P9">
         <f>N4*P4+N5*P5+N6*P6+N7*P7</f>
-        <v>360</v>
+        <v>450</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4">
-        <v>0</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="4">
-        <v>0</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="A11" s="5"/>
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="4">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="A12" s="5"/>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4">
-        <v>0</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="A13" s="5"/>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4">
-        <v>0</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="A14" s="5"/>
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="4">
-        <v>0</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="A15" s="5"/>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="4">
-        <v>0</v>
-      </c>
-      <c r="C16" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="4">
-        <v>0</v>
-      </c>
-      <c r="C17" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="4">
-        <v>0</v>
-      </c>
-      <c r="C21" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="4">
-        <v>0</v>
-      </c>
-      <c r="C22" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="4">
-        <v>0</v>
-      </c>
-      <c r="C23" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="4">
-        <v>0</v>
-      </c>
-      <c r="C24" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="4">
-        <v>0</v>
-      </c>
-      <c r="C25" s="5">
-        <v>0</v>
-      </c>
-      <c r="L25" s="6"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="4">
-        <v>0</v>
-      </c>
-      <c r="C26" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="4">
-        <v>0</v>
-      </c>
-      <c r="C27" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="4">
-        <v>0</v>
-      </c>
-      <c r="C28" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="4">
-        <v>0</v>
-      </c>
-      <c r="C29" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="4">
-        <v>0</v>
-      </c>
-      <c r="C30" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="4">
-        <v>0</v>
-      </c>
-      <c r="C31" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="4">
-        <v>0</v>
-      </c>
-      <c r="C32" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="4">
-        <v>0</v>
-      </c>
-      <c r="C33" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="4">
-        <v>0</v>
-      </c>
-      <c r="C34" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="4">
-        <v>0</v>
-      </c>
-      <c r="C35" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="4">
-        <v>0</v>
-      </c>
-      <c r="C36" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B39" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="3">
+        <v>0</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="3">
+        <v>0</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="5"/>
+      <c r="B35" s="3">
+        <v>0</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="5"/>
+      <c r="B36" s="3">
+        <v>0</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="4">
-        <v>0</v>
-      </c>
-      <c r="C40" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="4">
-        <v>0</v>
-      </c>
-      <c r="C41" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="4">
-        <v>0</v>
-      </c>
-      <c r="C42" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="4">
-        <v>0</v>
-      </c>
-      <c r="C43" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="4">
-        <v>0</v>
-      </c>
-      <c r="C44" s="5">
-        <v>0</v>
-      </c>
-      <c r="L44" s="6"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="4">
-        <v>0</v>
-      </c>
-      <c r="C45" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="4">
-        <v>0</v>
-      </c>
-      <c r="C46" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
-      <c r="B47" s="4">
-        <v>0</v>
-      </c>
-      <c r="C47" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-      <c r="B48" s="4">
-        <v>0</v>
-      </c>
-      <c r="C48" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
-      <c r="B49" s="4">
-        <v>0</v>
-      </c>
-      <c r="C49" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-      <c r="B50" s="4">
-        <v>0</v>
-      </c>
-      <c r="C50" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
-      <c r="B51" s="4">
-        <v>0</v>
-      </c>
-      <c r="C51" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
-      <c r="B52" s="4">
-        <v>0</v>
-      </c>
-      <c r="C52" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
-      <c r="B53" s="4">
-        <v>0</v>
-      </c>
-      <c r="C53" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
-      <c r="B54" s="4">
-        <v>0</v>
-      </c>
-      <c r="C54" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A55" s="2"/>
-      <c r="B55" s="4">
-        <v>0</v>
-      </c>
-      <c r="C55" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B58" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" s="3" t="s">
+      <c r="B40" s="3">
+        <v>0</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="5"/>
+      <c r="B41" s="3">
+        <v>0</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="5"/>
+      <c r="B42" s="3">
+        <v>0</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="5"/>
+      <c r="B43" s="3">
+        <v>0</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="5"/>
+      <c r="B44" s="3">
+        <v>0</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="5"/>
+      <c r="B45" s="3">
+        <v>0</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="5"/>
+      <c r="B46" s="3">
+        <v>0</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="5"/>
+      <c r="B47" s="3">
+        <v>0</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="5"/>
+      <c r="B48" s="3">
+        <v>0</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="5"/>
+      <c r="B49" s="3">
+        <v>0</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="5"/>
+      <c r="B50" s="3">
+        <v>0</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="5"/>
+      <c r="B51" s="3">
+        <v>0</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="5"/>
+      <c r="B52" s="3">
+        <v>0</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="5"/>
+      <c r="B53" s="3">
+        <v>0</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="5"/>
+      <c r="B54" s="3">
+        <v>0</v>
+      </c>
+      <c r="C54" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="5"/>
+      <c r="B55" s="3">
+        <v>0</v>
+      </c>
+      <c r="C55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B58" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="4">
-        <v>0</v>
-      </c>
-      <c r="C59" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A60" s="2"/>
-      <c r="B60" s="4">
-        <v>0</v>
-      </c>
-      <c r="C60" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
-      <c r="B61" s="4">
-        <v>0</v>
-      </c>
-      <c r="C61" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
-      <c r="B62" s="4">
-        <v>0</v>
-      </c>
-      <c r="C62" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
-      <c r="B63" s="4">
-        <v>0</v>
-      </c>
-      <c r="C63" s="5">
-        <v>0</v>
-      </c>
-      <c r="L63" s="6"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A64" s="2"/>
-      <c r="B64" s="4">
-        <v>0</v>
-      </c>
-      <c r="C64" s="5">
+      <c r="B59" s="3">
+        <v>0</v>
+      </c>
+      <c r="C59" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="5"/>
+      <c r="B60" s="3">
+        <v>0</v>
+      </c>
+      <c r="C60" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="5"/>
+      <c r="B61" s="3">
+        <v>0</v>
+      </c>
+      <c r="C61" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="5"/>
+      <c r="B62" s="3">
+        <v>0</v>
+      </c>
+      <c r="C62" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="5"/>
+      <c r="B63" s="3">
+        <v>0</v>
+      </c>
+      <c r="C63" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="5"/>
+      <c r="B64" s="3">
+        <v>0</v>
+      </c>
+      <c r="C64" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
-      <c r="B65" s="4">
-        <v>0</v>
-      </c>
-      <c r="C65" s="5">
+      <c r="A65" s="5"/>
+      <c r="B65" s="3">
+        <v>0</v>
+      </c>
+      <c r="C65" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="2"/>
-      <c r="B66" s="4">
-        <v>0</v>
-      </c>
-      <c r="C66" s="5">
+      <c r="A66" s="5"/>
+      <c r="B66" s="3">
+        <v>0</v>
+      </c>
+      <c r="C66" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
-      <c r="B67" s="4">
-        <v>0</v>
-      </c>
-      <c r="C67" s="5">
+      <c r="A67" s="5"/>
+      <c r="B67" s="3">
+        <v>0</v>
+      </c>
+      <c r="C67" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="2"/>
-      <c r="B68" s="4">
-        <v>0</v>
-      </c>
-      <c r="C68" s="5">
+      <c r="A68" s="5"/>
+      <c r="B68" s="3">
+        <v>0</v>
+      </c>
+      <c r="C68" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="2"/>
-      <c r="B69" s="4">
-        <v>0</v>
-      </c>
-      <c r="C69" s="5">
+      <c r="A69" s="5"/>
+      <c r="B69" s="3">
+        <v>0</v>
+      </c>
+      <c r="C69" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="2"/>
-      <c r="B70" s="4">
-        <v>0</v>
-      </c>
-      <c r="C70" s="5">
+      <c r="A70" s="5"/>
+      <c r="B70" s="3">
+        <v>0</v>
+      </c>
+      <c r="C70" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="2"/>
-      <c r="B71" s="4">
-        <v>0</v>
-      </c>
-      <c r="C71" s="5">
+      <c r="A71" s="5"/>
+      <c r="B71" s="3">
+        <v>0</v>
+      </c>
+      <c r="C71" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="2"/>
-      <c r="B72" s="4">
-        <v>0</v>
-      </c>
-      <c r="C72" s="5">
+      <c r="A72" s="5"/>
+      <c r="B72" s="3">
+        <v>0</v>
+      </c>
+      <c r="C72" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="2"/>
-      <c r="B73" s="4">
-        <v>0</v>
-      </c>
-      <c r="C73" s="5">
+      <c r="A73" s="5"/>
+      <c r="B73" s="3">
+        <v>0</v>
+      </c>
+      <c r="C73" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="2"/>
-      <c r="B74" s="4">
-        <v>0</v>
-      </c>
-      <c r="C74" s="5">
+      <c r="A74" s="5"/>
+      <c r="B74" s="3">
+        <v>0</v>
+      </c>
+      <c r="C74" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B77" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C77" s="3" t="s">
+      <c r="B77" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B78" s="4">
-        <v>0</v>
-      </c>
-      <c r="C78" s="5">
+      <c r="B78" s="3">
+        <v>0</v>
+      </c>
+      <c r="C78" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="2"/>
-      <c r="B79" s="4">
-        <v>0</v>
-      </c>
-      <c r="C79" s="5">
+      <c r="A79" s="5"/>
+      <c r="B79" s="3">
+        <v>0</v>
+      </c>
+      <c r="C79" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="2"/>
-      <c r="B80" s="4">
-        <v>0</v>
-      </c>
-      <c r="C80" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A81" s="2"/>
-      <c r="B81" s="4">
-        <v>0</v>
-      </c>
-      <c r="C81" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A82" s="2"/>
-      <c r="B82" s="4">
-        <v>0</v>
-      </c>
-      <c r="C82" s="5">
-        <v>0</v>
-      </c>
-      <c r="L82" s="6"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A83" s="2"/>
-      <c r="B83" s="4">
-        <v>0</v>
-      </c>
-      <c r="C83" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A84" s="2"/>
-      <c r="B84" s="4">
-        <v>0</v>
-      </c>
-      <c r="C84" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A85" s="2"/>
-      <c r="B85" s="4">
-        <v>0</v>
-      </c>
-      <c r="C85" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A86" s="2"/>
-      <c r="B86" s="4">
-        <v>0</v>
-      </c>
-      <c r="C86" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A87" s="2"/>
-      <c r="B87" s="4">
-        <v>0</v>
-      </c>
-      <c r="C87" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A88" s="2"/>
-      <c r="B88" s="4">
-        <v>0</v>
-      </c>
-      <c r="C88" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A89" s="2"/>
-      <c r="B89" s="4">
-        <v>0</v>
-      </c>
-      <c r="C89" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A90" s="2"/>
-      <c r="B90" s="4">
-        <v>0</v>
-      </c>
-      <c r="C90" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A91" s="2"/>
-      <c r="B91" s="4">
-        <v>0</v>
-      </c>
-      <c r="C91" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A92" s="2"/>
-      <c r="B92" s="4">
-        <v>0</v>
-      </c>
-      <c r="C92" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A93" s="2"/>
-      <c r="B93" s="4">
-        <v>0</v>
-      </c>
-      <c r="C93" s="5">
+      <c r="A80" s="5"/>
+      <c r="B80" s="3">
+        <v>0</v>
+      </c>
+      <c r="C80" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="5"/>
+      <c r="B81" s="3">
+        <v>0</v>
+      </c>
+      <c r="C81" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="5"/>
+      <c r="B82" s="3">
+        <v>0</v>
+      </c>
+      <c r="C82" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="5"/>
+      <c r="B83" s="3">
+        <v>0</v>
+      </c>
+      <c r="C83" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="5"/>
+      <c r="B84" s="3">
+        <v>0</v>
+      </c>
+      <c r="C84" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="5"/>
+      <c r="B85" s="3">
+        <v>0</v>
+      </c>
+      <c r="C85" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="5"/>
+      <c r="B86" s="3">
+        <v>0</v>
+      </c>
+      <c r="C86" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="5"/>
+      <c r="B87" s="3">
+        <v>0</v>
+      </c>
+      <c r="C87" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="5"/>
+      <c r="B88" s="3">
+        <v>0</v>
+      </c>
+      <c r="C88" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="5"/>
+      <c r="B89" s="3">
+        <v>0</v>
+      </c>
+      <c r="C89" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="5"/>
+      <c r="B90" s="3">
+        <v>0</v>
+      </c>
+      <c r="C90" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="5"/>
+      <c r="B91" s="3">
+        <v>0</v>
+      </c>
+      <c r="C91" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="5"/>
+      <c r="B92" s="3">
+        <v>0</v>
+      </c>
+      <c r="C92" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="5"/>
+      <c r="B93" s="3">
+        <v>0</v>
+      </c>
+      <c r="C93" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>